<commit_message>
Changes made for automating Wikipedia app
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TEST_DATA.xlsx
+++ b/src/test/resources/testdata/TEST_DATA.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\Projects\appium\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0224680D-0EBB-4B47-A914-76CBF35ABCDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A77117-F800-43F7-8080-240B7AE21217}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="702" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
-    <sheet name="ProductCatalog" sheetId="7" r:id="rId2"/>
+    <sheet name="HomeScreen" sheetId="7" r:id="rId2"/>
+    <sheet name="Login" sheetId="8" r:id="rId3"/>
+    <sheet name="Settings" sheetId="9" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -83,127 +85,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Pabba, Sagar:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-User Credentials to be used for submitting the request - gets resolved from Users Sheet</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Pabba, Sagar:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Name of the module under which the TC belons to &amp; in module named sheet there should be a entry detailing Test Data to be used.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Pabba, Sagar:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Specify which type of API to get invoked</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Pabba, Sagar:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Name of the template to refer under hierarchy
-src/test/resources/module</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Pabba, Sagar:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Use this column for marking TC dependency</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -242,8 +123,76 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Pabba, Sagar</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{E7FE9B78-8775-4A76-9B67-B54DB04A866F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Pabba, Sagar:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+TestCaseName same as the one defined in Base sheet</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Pabba, Sagar</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{ACD367C1-7739-4E0C-B9BA-C048CE1AEDD9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Pabba, Sagar:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+TestCaseName same as the one defined in Base sheet</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -266,9 +215,6 @@
     <t>Module</t>
   </si>
   <si>
-    <t>Operation</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -278,46 +224,52 @@
     <t>QA</t>
   </si>
   <si>
-    <t>Template</t>
-  </si>
-  <si>
-    <t>customerId</t>
-  </si>
-  <si>
-    <t>CCST_PROD</t>
-  </si>
-  <si>
-    <t>POST</t>
-  </si>
-  <si>
-    <t>DependsOn</t>
-  </si>
-  <si>
-    <t>User_Example</t>
-  </si>
-  <si>
-    <t>UserCredentialsID</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
-    <t>catalogName</t>
-  </si>
-  <si>
-    <t>RANDOM#CATALOG</t>
-  </si>
-  <si>
-    <t>Create_Catalog.json</t>
-  </si>
-  <si>
-    <t>Create a Catalog with End User</t>
-  </si>
-  <si>
-    <t>ProductCatalog</t>
-  </si>
-  <si>
-    <t>script1</t>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>test1automation</t>
+  </si>
+  <si>
+    <t>Appium@123</t>
+  </si>
+  <si>
+    <t>Verify the presence of icons present on the Home screen</t>
+  </si>
+  <si>
+    <t>verifyWelcomeScreenIcons</t>
+  </si>
+  <si>
+    <t>Verify the Login functionality</t>
+  </si>
+  <si>
+    <t>verifyLoginFunctionality</t>
+  </si>
+  <si>
+    <t>verifyLanguageSelectionFunctionality</t>
+  </si>
+  <si>
+    <t>Verify the Language selection functionality on Settings Screen</t>
+  </si>
+  <si>
+    <t>HomeScreen</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>Wikipedia Language</t>
+  </si>
+  <si>
+    <t>Simple English</t>
   </si>
 </sst>
 </file>
@@ -649,34 +601,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="1" max="1" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -694,54 +642,85 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -753,17 +732,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="53.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -775,32 +754,120 @@
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
         <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97482527-F40A-4A60-BE70-E97BA00FBA23}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{0875E835-736C-4F85-AFC7-01D7912B38B7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80CF02E6-0DAB-4F15-9F5E-389AAFA17FF1}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>